<commit_message>
Atualização para melhor legibilidade do código
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TopFama\Desktop\OPSender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TopFama\Documents\EnviadorMensagens\OPSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBBD05F-CC41-4669-8DB3-6E49C234EDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326C5AF3-8DA1-448C-968E-5DAEA2D39A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">teste </t>
-  </si>
-  <si>
-    <t>teste 2</t>
-  </si>
-  <si>
-    <t>teste 3</t>
-  </si>
-  <si>
-    <t>teste 4</t>
-  </si>
-  <si>
-    <t>teste 5</t>
-  </si>
-  <si>
-    <t>teste 6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Numero</t>
   </si>
@@ -69,10 +51,7 @@
     <t>teste 6.1</t>
   </si>
   <si>
-    <t>55 (63) 99212-2099</t>
-  </si>
-  <si>
-    <t>(63) 99212-2099</t>
+    <t>C:\Users\TopFama\Documents\EnviadorMensagens\OPSender\topfama_logo.png</t>
   </si>
 </sst>
 </file>
@@ -391,108 +370,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5563999514371</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>